<commit_message>
Fixed the error exception throwing stuff
</commit_message>
<xml_diff>
--- a/OGPC5 Game/Project Resources/Design/Towers vs. Enemies chart.xlsx
+++ b/OGPC5 Game/Project Resources/Design/Towers vs. Enemies chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="57">
   <si>
     <t>House</t>
   </si>
@@ -136,6 +136,57 @@
   </si>
   <si>
     <t>The ALT Money solution is so the game has even numbers, by 5's. Adjust the building prices because inflation.</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Armor damage</t>
+  </si>
+  <si>
+    <t>projectile Speed</t>
+  </si>
+  <si>
+    <t>Damage (per sec)</t>
+  </si>
+  <si>
+    <t>1 or 0</t>
+  </si>
+  <si>
+    <t>Fire Rate</t>
+  </si>
+  <si>
+    <t>Range(radius)</t>
+  </si>
+  <si>
+    <t>Happieness</t>
+  </si>
+  <si>
+    <t>One Half</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>Money Increase(per sec)</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>3 or 4</t>
+  </si>
+  <si>
+    <t>Damage(per sec)</t>
   </si>
 </sst>
 </file>
@@ -171,9 +222,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +541,10 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -759,216 +814,665 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>300</v>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J23" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B24">
-        <v>450</v>
+        <v>300</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>450</v>
       </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>150</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25">
+        <v>-2</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>500</v>
+        <v>450</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>150</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I26">
+        <v>-2</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>600</v>
+        <v>500</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>150</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27">
+        <v>-1</v>
+      </c>
+      <c r="J27">
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>1500</v>
+        <v>700</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>250</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28">
+        <v>-3</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>700</v>
+        <v>1500</v>
+      </c>
+      <c r="C29">
+        <v>35</v>
+      </c>
+      <c r="D29">
+        <v>500</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29">
+        <v>-2</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30">
-        <v>550</v>
+        <v>650</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>200</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>550</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>200</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>2000</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>31</v>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32">
+        <v>1000</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>10</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32">
+        <v>35</v>
+      </c>
+      <c r="J32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>50</v>
+      </c>
+      <c r="E36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
       <c r="B37">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C37">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
       <c r="B38">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>60</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
       <c r="B40">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>35</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B41">
-        <v>11</v>
+      <c r="B41" t="s">
+        <v>55</v>
       </c>
       <c r="C41">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>20</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>35</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>45</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
       <c r="B44">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>35</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
       <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>30</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>15</v>
+      </c>
+      <c r="C52">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>11</v>
       </c>
-      <c r="C45">
+      <c r="B53">
+        <v>13</v>
+      </c>
+      <c r="C53">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54">
+        <v>15</v>
+      </c>
+      <c r="C54">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55">
+        <v>13</v>
+      </c>
+      <c r="C55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59">
+        <v>12</v>
+      </c>
+      <c r="C59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+      <c r="C60">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enemies shoot now, but it's in progress
</commit_message>
<xml_diff>
--- a/OGPC5 Game/Project Resources/Design/Towers vs. Enemies chart.xlsx
+++ b/OGPC5 Game/Project Resources/Design/Towers vs. Enemies chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
   <si>
     <t>House</t>
   </si>
@@ -150,9 +150,6 @@
     <t>projectile Speed</t>
   </si>
   <si>
-    <t>Damage (per sec)</t>
-  </si>
-  <si>
     <t>1 or 0</t>
   </si>
   <si>
@@ -177,18 +174,9 @@
     <t>Money Increase(per sec)</t>
   </si>
   <si>
-    <t>Speed</t>
-  </si>
-  <si>
     <t>Armor</t>
   </si>
   <si>
-    <t>3 or 4</t>
-  </si>
-  <si>
-    <t>Damage(per sec)</t>
-  </si>
-  <si>
     <t>Range Coversion</t>
   </si>
   <si>
@@ -226,6 +214,15 @@
   </si>
   <si>
     <t>176 root(2)</t>
+  </si>
+  <si>
+    <t>Reload</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>very slow</t>
   </si>
 </sst>
 </file>
@@ -568,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,13 +862,13 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" t="s">
         <v>41</v>
@@ -880,16 +877,16 @@
         <v>42</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K23" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -909,13 +906,13 @@
         <v>2</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -924,10 +921,10 @@
         <v>3</v>
       </c>
       <c r="K24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -953,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I25">
         <v>-2</v>
@@ -962,10 +959,10 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -991,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I26">
         <v>-2</v>
@@ -1000,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1014,7 +1011,7 @@
         <v>500</v>
       </c>
       <c r="C27">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D27">
         <v>150</v>
@@ -1029,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I27">
         <v>-1</v>
@@ -1038,10 +1035,10 @@
         <v>7</v>
       </c>
       <c r="K27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1052,7 +1049,7 @@
         <v>700</v>
       </c>
       <c r="C28">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D28">
         <v>250</v>
@@ -1067,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I28">
         <v>-3</v>
@@ -1076,10 +1073,10 @@
         <v>2</v>
       </c>
       <c r="K28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1090,7 +1087,7 @@
         <v>1500</v>
       </c>
       <c r="C29">
-        <v>35</v>
+        <v>1000</v>
       </c>
       <c r="D29">
         <v>500</v>
@@ -1105,7 +1102,7 @@
         <v>0.5</v>
       </c>
       <c r="H29" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="I29">
         <v>-2</v>
@@ -1114,10 +1111,10 @@
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1143,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I30">
         <v>10</v>
@@ -1160,7 +1157,7 @@
         <v>550</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D31">
         <v>200</v>
@@ -1175,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I31">
         <v>8</v>
@@ -1192,7 +1189,7 @@
         <v>2000</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32">
         <v>1000</v>
@@ -1207,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I32">
         <v>35</v>
@@ -1218,16 +1215,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,10 +1232,10 @@
         <v>8</v>
       </c>
       <c r="B35">
+        <v>25</v>
+      </c>
+      <c r="C35">
         <v>2</v>
-      </c>
-      <c r="C35">
-        <v>3</v>
       </c>
       <c r="D35">
         <v>35</v>
@@ -1252,10 +1249,10 @@
         <v>9</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D36">
         <v>50</v>
@@ -1269,10 +1266,10 @@
         <v>10</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D37">
         <v>20</v>
@@ -1286,10 +1283,10 @@
         <v>11</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D38">
         <v>25</v>
@@ -1303,7 +1300,7 @@
         <v>12</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C39">
         <v>7</v>
@@ -1320,7 +1317,7 @@
         <v>13</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -1336,11 +1333,11 @@
       <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B41" t="s">
-        <v>54</v>
+      <c r="B41">
+        <v>50</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>20</v>
@@ -1354,10 +1351,10 @@
         <v>15</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>35</v>
@@ -1371,7 +1368,7 @@
         <v>16</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -1388,10 +1385,10 @@
         <v>20</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>35</v>
@@ -1405,7 +1402,7 @@
         <v>21</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C45">
         <v>3</v>

</xml_diff>

<commit_message>
You can't place roads on towers anymore!
</commit_message>
<xml_diff>
--- a/OGPC5 Game/Project Resources/Design/Towers vs. Enemies chart.xlsx
+++ b/OGPC5 Game/Project Resources/Design/Towers vs. Enemies chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
   <si>
     <t>House</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>very slow</t>
+  </si>
+  <si>
+    <t>Speed</t>
   </si>
 </sst>
 </file>
@@ -565,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>65</v>
       </c>
@@ -1226,8 +1229,11 @@
       <c r="E34" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1238,13 +1244,16 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1255,13 +1264,16 @@
         <v>10</v>
       </c>
       <c r="D36">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1272,13 +1284,16 @@
         <v>50</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="E37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1289,13 +1304,16 @@
         <v>15</v>
       </c>
       <c r="D38">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1306,13 +1324,16 @@
         <v>7</v>
       </c>
       <c r="D39">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E39">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -1323,13 +1344,16 @@
         <v>5</v>
       </c>
       <c r="D40">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1340,13 +1364,16 @@
         <v>5</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1357,13 +1384,16 @@
         <v>5</v>
       </c>
       <c r="D42">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1374,13 +1404,16 @@
         <v>4</v>
       </c>
       <c r="D43">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -1391,13 +1424,16 @@
         <v>5</v>
       </c>
       <c r="D44">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="E44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1408,13 +1444,16 @@
         <v>3</v>
       </c>
       <c r="D45">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E45">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>

</xml_diff>